<commit_message>
A Dog Said... Animal Prosthetics 2 update
asdf1
</commit_message>
<xml_diff>
--- a/Pull Request Here/A Dog Said2 - 3238353862/A Dog Said... Animal Prosthetics 2 - 3238353862.xlsx
+++ b/Pull Request Here/A Dog Said2 - 3238353862/A Dog Said... Animal Prosthetics 2 - 3238353862.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PDSSO2\Desktop\RimworldExtractor-Standard\RIM EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B7836F-F70B-4AF0-882D-E12BBBB23C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8593E1-DCFE-4D62-A4DA-87E5690FF1B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15" yWindow="225" windowWidth="22005" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5456,10 +5456,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>장착, 장착합니다, 설치 중</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>원래는 발볼록살이 맞습니다.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -5468,47 +5464,23 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>인게임에서 번역됐는지 확인부탁</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>모더의 실수(뇌절)이라고 봅니다.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>편의를 위해 비워두는게 좋아보임</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>("")는 쓸만한 한국어가 없었습니다.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>동물에게 이식할 때만 발톱으로 보임</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>&lt;-더 정확하고 좋은 번역이 필요합니다.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>인게임에서 번역되는지 확인하세요</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>림왈도에서는 귀만 '바이오겔'로 적습니다.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>&lt;- '신체부위'의 하위 카테고리</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>영문 설명에 없던 내용을 추가했습니다.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>아래는 EPOE 기존 번역본을 참고했습니다.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -5521,6 +5493,34 @@
 짐꾼이 될 수 있는 동물과 훈련 가능한 애완동물들 (집고양이 포함).
 이 기능을 비활성화하면 해당 동물들에게 적절한 수술을 수행할 수 있게 됩니다.
 재시작이 필요합니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;-영문 설명에 없던 내용을 추가했습니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>인게임에서 번역됐는지 확인해주세요.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>나중에 인게임에서 번역될지 확인하세요.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(동물에게 이식할 때만 발톱으로 보임)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(편의를 위해 비워두는게 좋아보임)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>[RMK] EPOE 기존 번역본을 참고했습니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(장착, 장착합니다, 설치 중)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -6234,7 +6234,7 @@
         <v>1173</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>1669</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -6526,7 +6526,7 @@
         <v>1600</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>1669</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -6682,7 +6682,7 @@
         <v>1188</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>1669</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -7195,7 +7195,7 @@
         <v>1204</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>1676</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
@@ -7626,7 +7626,7 @@
         <v>1214</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>1666</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
@@ -7714,7 +7714,7 @@
         <v>1486</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
@@ -8023,7 +8023,7 @@
         <v>1386</v>
       </c>
       <c r="G111" s="5" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
@@ -8043,7 +8043,7 @@
         <v>1387</v>
       </c>
       <c r="G112" s="5" t="s">
-        <v>1673</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -8876,7 +8876,7 @@
         <v>1587</v>
       </c>
       <c r="G161" s="5" t="s">
-        <v>1671</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.3">
@@ -8965,7 +8965,7 @@
         <v>1588</v>
       </c>
       <c r="G166" s="9" t="s">
-        <v>1677</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.3">
@@ -8985,7 +8985,7 @@
         <v>1663</v>
       </c>
       <c r="G167" s="5" t="s">
-        <v>1671</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.3">
@@ -9025,10 +9025,10 @@
         <v>1252</v>
       </c>
       <c r="F169" s="7" t="s">
-        <v>1680</v>
+        <v>1673</v>
       </c>
       <c r="G169" s="8" t="s">
-        <v>1674</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.3">
@@ -9975,7 +9975,7 @@
         <v>1285</v>
       </c>
       <c r="G216" s="5" t="s">
-        <v>1678</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.3">
@@ -11198,7 +11198,7 @@
         <v>1352</v>
       </c>
       <c r="G277" s="5" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.3">
@@ -11261,7 +11261,7 @@
         <v>1352</v>
       </c>
       <c r="G280" s="8" t="s">
-        <v>1669</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.3">
@@ -11444,7 +11444,7 @@
         <v>1344</v>
       </c>
       <c r="G289" s="8" t="s">
-        <v>1669</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.3">
@@ -11947,7 +11947,7 @@
         <v>1600</v>
       </c>
       <c r="G314" s="8" t="s">
-        <v>1669</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="315" spans="1:7" x14ac:dyDescent="0.3">
@@ -12390,7 +12390,7 @@
         <v>1397</v>
       </c>
       <c r="G336" s="5" t="s">
-        <v>1672</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="337" spans="1:6" x14ac:dyDescent="0.3">
@@ -13573,7 +13573,7 @@
         <v>1640</v>
       </c>
       <c r="G395" s="8" t="s">
-        <v>1674</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="396" spans="1:7" x14ac:dyDescent="0.3">
@@ -13928,7 +13928,7 @@
         <v>1027</v>
       </c>
       <c r="G412" s="5" t="s">
-        <v>1670</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="413" spans="1:7" x14ac:dyDescent="0.3">
@@ -13966,7 +13966,7 @@
         <v>1593</v>
       </c>
       <c r="G414" s="8" t="s">
-        <v>1675</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="415" spans="1:7" x14ac:dyDescent="0.3">
@@ -14079,7 +14079,7 @@
         <v>1655</v>
       </c>
       <c r="G420" s="8" t="s">
-        <v>1674</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="421" spans="1:7" x14ac:dyDescent="0.3">
@@ -14260,7 +14260,7 @@
         <v>1064</v>
       </c>
       <c r="G429" s="5" t="s">
-        <v>1670</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="430" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>